<commit_message>
Completo Api Controller Bancos
</commit_message>
<xml_diff>
--- a/SQLServer.xlsx
+++ b/SQLServer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesarrolloIntegral\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B2E97-0B6C-40E4-8641-F249458E5CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4775A24-56E5-4C1F-9A70-FE778F932878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{908AB308-4C8D-46BE-BEF3-E86EB363CC25}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>IdCuenta</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Identity</t>
+  </si>
+  <si>
+    <t>tbBanco</t>
+  </si>
+  <si>
+    <t>IdBanco</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -406,51 +418,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DB2D41-FA4B-4D27-8724-B9D97F8B1E8A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="C10">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>